<commit_message>
Cleaned up bike template spreadsheet.
</commit_message>
<xml_diff>
--- a/output_templates/Bike_Template.xlsx
+++ b/output_templates/Bike_Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="82">
   <si>
     <t>hhno</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Age Group</t>
   </si>
   <si>
-    <t>this isn't ordered needs some coding here</t>
-  </si>
-  <si>
     <t>Mode Shares, Persons, Purpose, and Destination</t>
   </si>
   <si>
@@ -250,6 +247,21 @@
   </si>
   <si>
     <t>Bike Trip Lengths by Destination District</t>
+  </si>
+  <si>
+    <t>Bike Mode Share by Trip Purpose</t>
+  </si>
+  <si>
+    <t>Bike Mode Share by Destination County</t>
+  </si>
+  <si>
+    <t>Bike Mode Share by Destination District</t>
+  </si>
+  <si>
+    <t>Bike Mode Share by Gender</t>
+  </si>
+  <si>
+    <t>Bike Mode Share by Age Grou</t>
   </si>
 </sst>
 </file>
@@ -501,9 +513,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -519,7 +530,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Summary!$H$6:$H$21</c:f>
@@ -577,6 +587,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -592,7 +603,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Summary!$J$6:$J$21</c:f>
@@ -646,6 +656,254 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>4.7936085219707054E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="164705792"/>
+        <c:axId val="164707328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="164705792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164707328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="164707328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164705792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$7:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Escort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Meal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>None/Home</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Personal Business</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>School</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shop</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Social</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.5356132681923372E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.083907839258238E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1878888460203688E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7465110262224723E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7585845896147404E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8392874912926667E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.735340838455694E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3016900395541172E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$7:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Escort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Meal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>None/Home</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Personal Business</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>School</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shop</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Social</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$7:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2278645830077338E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6054950507269567E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1219856861985806E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9818178965079568E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6526062615157409E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4926288447098179E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9968371920323514E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5092049598227167E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,11 +918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="178447488"/>
-        <c:axId val="178890240"/>
+        <c:axId val="88651264"/>
+        <c:axId val="88652800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="178447488"/>
+        <c:axId val="88651264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178890240"/>
+        <c:crossAx val="88652800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -681,18 +939,1593 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178890240"/>
+        <c:axId val="88652800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178447488"/>
+        <c:crossAx val="88651264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$17:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0860241024060763E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2082251444844627E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0575829522300982E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.014124917236813E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$17:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1204845519965019E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.419438068857702E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4509170891778305E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6488444285143829E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="84951424"/>
+        <c:axId val="84952960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="84951424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84952960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84952960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84951424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$23:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>East Side</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Everett-Lynwood-Edmonds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>North Seattle-Shoreline</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Renton-FedWay-Kent</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S.Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seattle CBD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>South Pierce</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Suburban Snohomish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tacoma</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>West-South Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$23:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0447586171514846E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1140535857322675E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2082251444844627E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1750784509035897E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8829116025768741E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6437709112379456E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5701434375259098E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0217345480947139E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3235416081437188E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1378078435689339E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0890699983451928E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$23:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>East Side</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Everett-Lynwood-Edmonds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>North Seattle-Shoreline</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Renton-FedWay-Kent</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S.Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seattle CBD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>South Pierce</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Suburban Snohomish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tacoma</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>West-South Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$23:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.0625606366643149E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8632166536354887E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.419438068857702E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9986169607678732E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0904430172142128E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4477668636269657E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2057684970154075E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4138374858645806E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9320529436393813E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="88360832"/>
+        <c:axId val="88362368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="88360832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88362368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88362368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88360832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$35:$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$36:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.9980151864353661E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8060438687469748E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$35:$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$37:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.3629884257838343E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3551232852431523E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90723456"/>
+        <c:axId val="90724992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90723456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90724992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90724992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90723456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$40:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>(0, 16]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(16, 35]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(35, 64]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(64, 80]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$40:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.8555658770199344E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1399871131891552E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7902264600715138E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9674424274438493E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey Bike Share</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$40:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>(0, 16]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(16, 35]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(35, 64]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(64, 80]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$40:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.3212352753900031E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0756782484531175E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1875284248825104E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0802741067058247E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="79442304"/>
+        <c:axId val="80740352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79442304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80740352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80740352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79442304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$24:$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Escort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Meal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>None/Home</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Personal Business</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>School</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shop</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Social</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$G$24:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.5276837663911795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.71513743388397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4220280299481702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.49759040916036</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5656031734997198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5857557215039102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1029777335532902</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.8251998679316204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$H$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$24:$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Escort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Meal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>None/Home</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Personal Business</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>School</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shop</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Social</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$H$24:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5578834899829999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6977820296136308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0855419253275604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0267036961239304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8654899658603701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6802366459092499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8548115634528699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7926836775240194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="85740544"/>
+        <c:axId val="88023808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85740544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88023808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88023808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85740544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$G$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$35:$F$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$G$35:$G$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.3115575267502901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9360617442580002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8684977314109199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7738249452211798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$H$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$35:$F$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$H$35:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.3198551202207698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0686691771339296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8761342573331801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9895852414735198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="93444352"/>
+        <c:axId val="93499392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93444352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93499392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93499392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93444352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$G$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$41:$F$51</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>East Side</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Everett-Lynwood-Edmonds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>North Seattle-Shoreline</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Renton-FedWay-Kent</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S.Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seattle CBD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>South Pierce</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Suburban Snohomish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tacoma</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>West-South Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$G$41:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.2966471329030798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6909301039373998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9360617442580002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3108371200887099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8043219298782303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8013010770459701</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2665974504283799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8420964651674199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8548763574663303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.74821695203575</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8549939406577796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$H$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Survey</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$F$41:$F$51</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>East Side</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Everett-Lynwood-Edmonds</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>North Seattle-Shoreline</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Renton-FedWay-Kent</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S.Kitsap</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seattle CBD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>South Pierce</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Suburban Snohomish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tacoma</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>West-South Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$H$41:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6.8312608225968603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5332809197486501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0686691771339296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.59305279779749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.96328058057586</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5177921420600402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.39826269692339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3166612441623498</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4402761308988099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2392745569377901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90739456"/>
+        <c:axId val="90740992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90739456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90740992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90740992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90739456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -719,15 +2552,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -741,6 +2574,246 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>195262</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1039,7 +3112,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +3133,7 @@
         <v>9.3395676199274427E-3</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="26">
         <f>BikeRawData!B216</f>
@@ -1076,7 +3149,7 @@
         <v>1.0752480135565177E-2</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="26">
         <f>BikeRawData!B215</f>
@@ -1086,33 +3159,36 @@
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>64</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
       <c r="F5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="14" t="s">
         <v>70</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1392,7 +3468,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F15" s="29">
         <v>9</v>
       </c>
@@ -1564,6 +3642,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
       <c r="F21" s="30">
         <v>15</v>
       </c>
@@ -1607,13 +3688,13 @@
         <v>8.0625606366643149E-3</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,10 +3810,7 @@
         <f>BikeRawData!B101/BikeRawData!B121</f>
         <v>9.6437709112379456E-3</v>
       </c>
-      <c r="C28" s="10">
-        <f>BikeRawData!B141/BikeRawData!B161</f>
-        <v>7.5459572959035479E-2</v>
-      </c>
+      <c r="C28" s="10"/>
       <c r="F28" s="8" t="str">
         <f>BikeRawData!A265</f>
         <v>School</v>
@@ -1853,15 +3931,17 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="F34" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,7 +4020,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F38" s="11" t="str">
         <f>BikeRawData!A288</f>
@@ -1972,21 +4052,21 @@
         <v>(0, 16]</v>
       </c>
       <c r="B40" s="9">
-        <f>BikeRawData!B191/BikeRawData!B199</f>
+        <f>SUMIF(BikeRawData!$A$191:$A$194,Summary!$A40,BikeRawData!$B$191:$B$194)/SUMIF(BikeRawData!$A$197:$A$200,Summary!$A40,BikeRawData!$B$197:$B$200)</f>
         <v>1.8555658770199344E-2</v>
       </c>
       <c r="C40" s="10">
-        <f>BikeRawData!B204/BikeRawData!B210</f>
+        <f>SUMIF(BikeRawData!$A$203:$A$206,Summary!$A40,BikeRawData!$B$203:$B$206)/SUMIF(BikeRawData!$A$209:$A$212,Summary!A40,BikeRawData!$B$209:$B$212)</f>
         <v>1.3212352753900031E-2</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1995,11 +4075,11 @@
         <v>(16, 35]</v>
       </c>
       <c r="B41" s="9">
-        <f>BikeRawData!B193/BikeRawData!B198</f>
+        <f>SUMIF(BikeRawData!$A$191:$A$194,Summary!$A41,BikeRawData!$B$191:$B$194)/SUMIF(BikeRawData!$A$197:$A$200,Summary!$A41,BikeRawData!$B$197:$B$200)</f>
         <v>1.1399871131891552E-2</v>
       </c>
       <c r="C41" s="10">
-        <f>BikeRawData!B205/BikeRawData!B211</f>
+        <f>SUMIF(BikeRawData!$A$203:$A$206,Summary!$A41,BikeRawData!$B$203:$B$206)/SUMIF(BikeRawData!$A$209:$A$212,Summary!A41,BikeRawData!$B$209:$B$212)</f>
         <v>1.0756782484531175E-2</v>
       </c>
       <c r="F41" s="8" t="str">
@@ -2020,11 +4100,11 @@
         <v>33</v>
       </c>
       <c r="B42" s="9">
-        <f>BikeRawData!B192/BikeRawData!B197</f>
+        <f>SUMIF(BikeRawData!$A$191:$A$194,Summary!$A42,BikeRawData!$B$191:$B$194)/SUMIF(BikeRawData!$A$197:$A$200,Summary!$A42,BikeRawData!$B$197:$B$200)</f>
         <v>7.7902264600715138E-3</v>
       </c>
       <c r="C42" s="10">
-        <f>BikeRawData!B203/BikeRawData!B209</f>
+        <f>SUMIF(BikeRawData!$A$203:$A$206,Summary!$A42,BikeRawData!$B$203:$B$206)/SUMIF(BikeRawData!$A$209:$A$212,Summary!A42,BikeRawData!$B$209:$B$212)</f>
         <v>1.1875284248825104E-2</v>
       </c>
       <c r="F42" s="8" t="str">
@@ -2046,11 +4126,11 @@
         <v>(64, 80]</v>
       </c>
       <c r="B43" s="12">
-        <f>BikeRawData!B194/BikeRawData!B200</f>
+        <f>SUMIF(BikeRawData!$A$191:$A$194,Summary!$A43,BikeRawData!$B$191:$B$194)/SUMIF(BikeRawData!$A$197:$A$200,Summary!$A43,BikeRawData!$B$197:$B$200)</f>
         <v>4.9674424274438493E-3</v>
       </c>
       <c r="C43" s="13">
-        <f>BikeRawData!B206/BikeRawData!B212</f>
+        <f>SUMIF(BikeRawData!$A$203:$A$206,Summary!$A43,BikeRawData!$B$203:$B$206)/SUMIF(BikeRawData!$A$209:$A$212,Summary!A43,BikeRawData!$B$209:$B$212)</f>
         <v>2.0802741067058247E-3</v>
       </c>
       <c r="F43" s="8" t="str">
@@ -2189,10 +4269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C326"/>
+  <dimension ref="A2:E326"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259"/>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="N243" sqref="N243:O243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,7 +5493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>41</v>
       </c>
@@ -3424,7 +5504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>42</v>
       </c>
@@ -3435,7 +5515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>43</v>
       </c>
@@ -3446,7 +5526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>44</v>
       </c>
@@ -3457,7 +5537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>45</v>
       </c>
@@ -3468,7 +5548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>46</v>
       </c>
@@ -3479,7 +5559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>47</v>
       </c>
@@ -3490,7 +5570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>48</v>
       </c>
@@ -3501,7 +5581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>49</v>
       </c>
@@ -3512,7 +5592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>50</v>
       </c>
@@ -3523,7 +5603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>51</v>
       </c>
@@ -3534,17 +5614,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B239" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B240" s="1">
         <v>147</v>
+      </c>
+      <c r="E240" s="1" t="str">
+        <f>RIGHT(A240, 4)</f>
+        <v>, 3]</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>